<commit_message>
introdução do metodo hooke
</commit_message>
<xml_diff>
--- a/aterramento/tabelaExemplo2_12GeraldoKindermann.xlsx
+++ b/aterramento/tabelaExemplo2_12GeraldoKindermann.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14640" windowHeight="5100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14640" windowHeight="5100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tabelaResistividadeMedida" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <t>E</t>
   </si>
   <si>
-    <t>profundidade do cravamento (m)</t>
+    <t>profundidade de cravamento (m)</t>
   </si>
 </sst>
 </file>
@@ -122,10 +122,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -410,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,19 +420,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -583,9 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>